<commit_message>
Updated Readme to include app instructions Added new images to readme Updated manual testing excel spreadsheet Included a PDF guide to my manual testing
</commit_message>
<xml_diff>
--- a/manualtesting.xlsx
+++ b/manualtesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucy.THEASHNETWORK\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\lucyshepherd\repos\assignment-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26014F0-AFFD-4022-ADD9-EC70BFB42738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B561C501-C39E-4632-BE8B-A95FB7CD8493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14520" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{BF2E4271-B390-4CB9-8EC6-0600AC412001}"/>
+    <workbookView xWindow="14280" yWindow="-16335" windowWidth="29040" windowHeight="15720" xr2:uid="{BF2E4271-B390-4CB9-8EC6-0600AC412001}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
   <si>
     <t>Function Tested</t>
   </si>
@@ -60,15 +60,6 @@
     <t>Confirm recipe is added successfully</t>
   </si>
   <si>
-    <t>Check the added recipe appears in the selected category</t>
-  </si>
-  <si>
-    <t>Modify recipe</t>
-  </si>
-  <si>
-    <t>Modify a current recipe</t>
-  </si>
-  <si>
     <t>Choose "modify recipe"</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Confirm recipe is successfully modified</t>
   </si>
   <si>
-    <t>Delete a recipe</t>
-  </si>
-  <si>
     <t>Choose "delete recipe"</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>Confirm deletion</t>
   </si>
   <si>
-    <t>Check the details have been modified correctly</t>
-  </si>
-  <si>
     <t>Verify details are displayed correctly</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>Choose "search recipe"</t>
   </si>
   <si>
-    <t>Enter ingredient name present in 2 or more recipes</t>
-  </si>
-  <si>
     <t>Check they are sorted alphabetically</t>
   </si>
   <si>
@@ -132,21 +114,6 @@
     <t>Confirm a PDF file is created with correct recipe details</t>
   </si>
   <si>
-    <t>Input or exit</t>
-  </si>
-  <si>
-    <t>Check user can exit at each input</t>
-  </si>
-  <si>
-    <t>Select category and enter "exit" for recipe name</t>
-  </si>
-  <si>
-    <t>Confirm exit to main menu</t>
-  </si>
-  <si>
-    <t>Repeat for method and ingredients</t>
-  </si>
-  <si>
     <t>Runs without errors</t>
   </si>
   <si>
@@ -159,36 +126,15 @@
     <t>Receive "Recipe added successfully!" message</t>
   </si>
   <si>
-    <t>Add recipe + View Recipe</t>
-  </si>
-  <si>
     <t>Add 5 recipes, check they've been added to desired category</t>
   </si>
   <si>
-    <t>Recipe shows in desired category and displays when selected</t>
-  </si>
-  <si>
     <t>Repeat - add 5 recipes that share a common ingredient</t>
   </si>
   <si>
     <t>All 5 recipes added without error</t>
   </si>
   <si>
-    <t>Allows you to exit when entered without errors</t>
-  </si>
-  <si>
-    <t>Exits back to main menu</t>
-  </si>
-  <si>
-    <t>Works for recipe name/ ingredients/ method</t>
-  </si>
-  <si>
-    <t>Check no unwanted items have been added to DB</t>
-  </si>
-  <si>
-    <t>Any items entered before 'exit' don't exist</t>
-  </si>
-  <si>
     <t>Displays recipe and prompts you to select what to modify</t>
   </si>
   <si>
@@ -198,18 +144,12 @@
     <t>Modified detail is now displayed when viewing recipe</t>
   </si>
   <si>
-    <t>Item modified has been replaced with new value in DB</t>
-  </si>
-  <si>
     <t>Displays "recipe has been deleted"</t>
   </si>
   <si>
     <t>No longer in category or DB</t>
   </si>
   <si>
-    <t>Delete recipe + select category empty</t>
-  </si>
-  <si>
     <t xml:space="preserve">View empty category </t>
   </si>
   <si>
@@ -244,13 +184,79 @@
   </si>
   <si>
     <t>3 files successful, 1 encountered UnicodeError</t>
+  </si>
+  <si>
+    <t>Check DB is created if it doesn't already exist</t>
+  </si>
+  <si>
+    <t>DB is created</t>
+  </si>
+  <si>
+    <t>Check exit function for each input prompt</t>
+  </si>
+  <si>
+    <t>Check duplicate recipe names can't be added</t>
+  </si>
+  <si>
+    <t>Check symbols can be used without returning an error</t>
+  </si>
+  <si>
+    <t>Exit to main menu with no errors</t>
+  </si>
+  <si>
+    <t>Returns error asking for unique name</t>
+  </si>
+  <si>
+    <t>Allows special characters without error</t>
+  </si>
+  <si>
+    <t>Modify recipe, delete recipe, view recipe</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Add recipe, view recipe</t>
+  </si>
+  <si>
+    <t>View each newly added recipe</t>
+  </si>
+  <si>
+    <t>Prints recipes to screen without error</t>
+  </si>
+  <si>
+    <t>Testing DB retrieval/modify features</t>
+  </si>
+  <si>
+    <t>Enter common ingredient (test upper and lower)</t>
+  </si>
+  <si>
+    <t>Search for non-existant ingredient</t>
+  </si>
+  <si>
+    <t>Displays 0 search result error</t>
+  </si>
+  <si>
+    <t>Test empty search</t>
+  </si>
+  <si>
+    <t>Asks for user input</t>
+  </si>
+  <si>
+    <t>Search for a special symbol</t>
+  </si>
+  <si>
+    <t>Returns results without an error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +268,15 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,6 +469,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A44D35-BFC4-4D11-AB92-66FDC5DD80CD}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,10 +835,10 @@
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="7"/>
@@ -831,10 +855,10 @@
         <v>7</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G3" s="11"/>
     </row>
@@ -847,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -860,13 +884,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G5" s="11"/>
     </row>
@@ -876,29 +900,29 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="C7" s="19">
-        <v>5</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>46</v>
+      <c r="E7" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
       </c>
       <c r="G7" s="11"/>
     </row>
@@ -908,516 +932,424 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24"/>
+      <c r="C11" s="19">
+        <v>9</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="C12" s="19">
+        <v>10</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="C11" s="1">
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="C15" s="19">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="C12" s="1">
+      <c r="D15" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="C16" s="1">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="C13" s="1">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="C14" s="1">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="C15" s="1">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="9"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19">
+        <v>4</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
-      <c r="C19" s="19">
-        <v>3</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>54</v>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
       </c>
       <c r="G19" s="11"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:7" s="18" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="C22" s="19">
-        <v>6</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="9"/>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="C24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="C25" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F25" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
-      <c r="C27" s="1">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" t="s">
-        <v>59</v>
+      <c r="C27" s="19">
+        <v>5</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
-      <c r="B28" s="18"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
       <c r="C28" s="19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>41</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E28" s="22"/>
       <c r="F28" s="23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="9"/>
+      <c r="A29" s="10"/>
+      <c r="C29" s="19">
+        <v>7</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F30" t="s">
-        <v>40</v>
+      <c r="C30" s="19">
+        <v>8</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="C31" s="1">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="11"/>
+      <c r="A31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="C32" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="C33" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14">
+        <v>3</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="C34" s="1">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="C35" s="19">
-        <v>6</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" t="s">
-        <v>40</v>
-      </c>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" t="s">
-        <v>68</v>
-      </c>
-      <c r="G38" s="11"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="C39" s="1">
-        <v>3</v>
-      </c>
-      <c r="D39" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14">
-        <v>4</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40" s="15" t="s">
-        <v>72</v>
+      <c r="E34" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>